<commit_message>
Added figures to paper
</commit_message>
<xml_diff>
--- a/Paper/Experiments.xlsx
+++ b/Paper/Experiments.xlsx
@@ -16,48 +16,72 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Error</t>
   </si>
   <si>
-    <t>0.5 Error</t>
+    <t># Training</t>
   </si>
   <si>
-    <t>1 Error</t>
+    <t>1 Tree</t>
   </si>
   <si>
-    <t>10 Error</t>
+    <t>2 Trees</t>
   </si>
   <si>
-    <t>20 Error</t>
+    <t>3 Trees</t>
   </si>
   <si>
-    <t>40 Error</t>
+    <t>4 Trees</t>
   </si>
   <si>
-    <t>60 Error</t>
+    <t>5 Trees</t>
   </si>
   <si>
-    <t>100 Error</t>
+    <t>1000 Features</t>
   </si>
   <si>
-    <t>200 Error</t>
+    <t>2000 Features</t>
   </si>
   <si>
-    <t>3000 Error</t>
+    <t>3000 Features</t>
   </si>
   <si>
-    <t>2000 Error</t>
+    <t>Training accuracy</t>
   </si>
   <si>
-    <t>1000 Error</t>
+    <t>Test accuracy</t>
   </si>
   <si>
-    <t># Trees</t>
+    <t>Random forest</t>
   </si>
   <si>
-    <t># Training</t>
+    <t>Linear SVM</t>
+  </si>
+  <si>
+    <t>1000 mmpx</t>
+  </si>
+  <si>
+    <t>2000 mmpx</t>
+  </si>
+  <si>
+    <t>20000 mmpx</t>
+  </si>
+  <si>
+    <t>40000 mmpx</t>
+  </si>
+  <si>
+    <t>80000 mmpx</t>
+  </si>
+  <si>
+    <t>120000 mmpx</t>
+  </si>
+  <si>
+    <t>200000 mmpx</t>
+  </si>
+  <si>
+    <t>400000 mmpx</t>
   </si>
 </sst>
 </file>
@@ -130,69 +154,244 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$B$1</c:f>
+              <c:f>Data!$S$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Error</c:v>
+                  <c:v>1 Tree</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Data!$A$2:$A$7</c:f>
+              <c:f>Data!$S$13:$S$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.36840000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0.22409999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0.1822</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0.12759999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>0.1237</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>8.3799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.6999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.1500000000000003E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$T$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2 Trees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$7</c:f>
+              <c:f>Data!$T$13:$T$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8.1500000000000003E-2</c:v>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.37380000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.22670000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18720000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1234</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7599999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3500000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.4700000000000003E-2</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$U$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3 Trees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$U$13:$U$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23949999999999999</c:v>
+                </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.18229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.2499999999999995E-2</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$V$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4 Trees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$V$13:$V$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.36770000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1855</c:v>
+                </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.12130000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1268</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1800000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.5499999999999998E-2</c:v>
                 </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$W$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5 Trees</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$W$13:$W$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.36899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24560000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18179999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1206</c:v>
+                </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.12529999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4299999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4500000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>7.7439999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.4000000000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -209,11 +408,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="120577024"/>
-        <c:axId val="66110592"/>
+        <c:axId val="96103424"/>
+        <c:axId val="96105600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="120577024"/>
+        <c:axId val="96103424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -242,7 +441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66110592"/>
+        <c:crossAx val="96105600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -250,7 +449,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="66110592"/>
+        <c:axId val="96105600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -282,11 +481,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120577024"/>
+        <c:crossAx val="96103424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -328,7 +532,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1000 Error</c:v>
+                  <c:v>1000 Features</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -410,7 +614,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2000 Error</c:v>
+                  <c:v>2000 Features</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -459,7 +663,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3000 Error</c:v>
+                  <c:v>3000 Features</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -509,11 +713,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68442368"/>
-        <c:axId val="68448640"/>
+        <c:axId val="100546816"/>
+        <c:axId val="100548992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68442368"/>
+        <c:axId val="100546816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -542,7 +746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68448640"/>
+        <c:crossAx val="100548992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -550,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68448640"/>
+        <c:axId val="100548992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -582,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68442368"/>
+        <c:crossAx val="100546816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -722,11 +926,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="68501888"/>
-        <c:axId val="68503808"/>
+        <c:axId val="100565376"/>
+        <c:axId val="100567296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="68501888"/>
+        <c:axId val="100565376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68503808"/>
+        <c:crossAx val="100567296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -763,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68503808"/>
+        <c:axId val="100567296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -795,7 +999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="68501888"/>
+        <c:crossAx val="100565376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -841,7 +1045,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.5 Error</c:v>
+                  <c:v>1000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -923,7 +1127,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1 Error</c:v>
+                  <c:v>2000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1005,7 +1209,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10 Error</c:v>
+                  <c:v>20000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1087,7 +1291,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20 Error</c:v>
+                  <c:v>40000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1169,7 +1373,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>40 Error</c:v>
+                  <c:v>80000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1251,7 +1455,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>60 Error</c:v>
+                  <c:v>120000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1333,7 +1537,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>100 Error</c:v>
+                  <c:v>200000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1415,7 +1619,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>200 Error</c:v>
+                  <c:v>400000 mmpx</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1498,11 +1702,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89333120"/>
-        <c:axId val="91428352"/>
+        <c:axId val="105213312"/>
+        <c:axId val="105219584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89333120"/>
+        <c:axId val="105213312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1531,7 +1735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="91428352"/>
+        <c:crossAx val="105219584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1539,7 +1743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91428352"/>
+        <c:axId val="105219584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -1571,7 +1775,453 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89333120"/>
+        <c:crossAx val="105213312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$S$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Training accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$S$26:$S$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8.8999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.23E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.15E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.06E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.2999999999999992E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$T$25</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Test accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$T$26:$T$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2499999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="116587136"/>
+        <c:axId val="116622080"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="116587136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of trees</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="116622080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="116622080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="116587136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$S$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random forest</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$S$42:$S$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.371</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18229999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12239999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.2900000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2499999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$T$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Linear SVM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$T$42:$T$49</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.56499999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52500000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.503</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.495</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.497</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="113098112"/>
+        <c:axId val="113763840"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="113098112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of trees</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113763840"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="113763840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Error</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113098112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1716,6 +2366,70 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2011,10 +2725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+  <dimension ref="D1:W49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,68 +2738,61 @@
     <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="R1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="S1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>8.1500000000000003E-2</v>
-      </c>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D2">
         <v>10</v>
       </c>
@@ -2132,13 +2839,7 @@
         <v>0.42620000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>7.4700000000000003E-2</v>
-      </c>
+    <row r="3" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>50</v>
       </c>
@@ -2185,13 +2886,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>7.2499999999999995E-2</v>
-      </c>
+    <row r="4" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>100</v>
       </c>
@@ -2238,13 +2933,7 @@
         <v>0.31859999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>7.5499999999999998E-2</v>
-      </c>
+    <row r="5" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>150</v>
       </c>
@@ -2291,13 +2980,7 @@
         <v>0.24349999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>7.7439999999999995E-2</v>
-      </c>
+    <row r="6" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>200</v>
       </c>
@@ -2344,13 +3027,7 @@
         <v>0.24079999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>8.4000000000000005E-2</v>
-      </c>
+    <row r="7" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>250</v>
       </c>
@@ -2397,7 +3074,7 @@
         <v>0.2316</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>300</v>
       </c>
@@ -2444,7 +3121,7 @@
         <v>0.20519999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>350</v>
       </c>
@@ -2491,12 +3168,390 @@
         <v>0.18509999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I10">
         <v>689</v>
       </c>
       <c r="J10">
         <v>1.32E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="R12" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" t="s">
+        <v>3</v>
+      </c>
+      <c r="U12" t="s">
+        <v>4</v>
+      </c>
+      <c r="V12" t="s">
+        <v>5</v>
+      </c>
+      <c r="W12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>10</v>
+      </c>
+      <c r="S13">
+        <v>0.36840000000000001</v>
+      </c>
+      <c r="T13">
+        <v>0.37380000000000002</v>
+      </c>
+      <c r="U13">
+        <v>0.371</v>
+      </c>
+      <c r="V13">
+        <v>0.36770000000000003</v>
+      </c>
+      <c r="W13">
+        <v>0.36899999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>50</v>
+      </c>
+      <c r="S14">
+        <v>0.22409999999999999</v>
+      </c>
+      <c r="T14">
+        <v>0.22670000000000001</v>
+      </c>
+      <c r="U14">
+        <v>0.23949999999999999</v>
+      </c>
+      <c r="V14">
+        <v>0.24329999999999999</v>
+      </c>
+      <c r="W14">
+        <v>0.24560000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>100</v>
+      </c>
+      <c r="S15">
+        <v>0.1822</v>
+      </c>
+      <c r="T15">
+        <v>0.18720000000000001</v>
+      </c>
+      <c r="U15">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="V15">
+        <v>0.1855</v>
+      </c>
+      <c r="W15">
+        <v>0.18179999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>150</v>
+      </c>
+      <c r="S16">
+        <v>0.12759999999999999</v>
+      </c>
+      <c r="T16">
+        <v>0.12859999999999999</v>
+      </c>
+      <c r="U16">
+        <v>0.12239999999999999</v>
+      </c>
+      <c r="V16">
+        <v>0.12130000000000001</v>
+      </c>
+      <c r="W16">
+        <v>0.1206</v>
+      </c>
+    </row>
+    <row r="17" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>200</v>
+      </c>
+      <c r="S17">
+        <v>0.1237</v>
+      </c>
+      <c r="T17">
+        <v>0.1234</v>
+      </c>
+      <c r="U17">
+        <v>0.1303</v>
+      </c>
+      <c r="V17">
+        <v>0.1268</v>
+      </c>
+      <c r="W17">
+        <v>0.12529999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>250</v>
+      </c>
+      <c r="S18">
+        <v>8.3799999999999999E-2</v>
+      </c>
+      <c r="T18">
+        <v>8.7599999999999997E-2</v>
+      </c>
+      <c r="U18">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="V18">
+        <v>9.1800000000000007E-2</v>
+      </c>
+      <c r="W18">
+        <v>9.4299999999999995E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>300</v>
+      </c>
+      <c r="S19">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="T19">
+        <v>8.3500000000000005E-2</v>
+      </c>
+      <c r="U19">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="V19">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="W19">
+        <v>8.4500000000000006E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>350</v>
+      </c>
+      <c r="S20">
+        <v>8.1500000000000003E-2</v>
+      </c>
+      <c r="T20">
+        <v>7.4700000000000003E-2</v>
+      </c>
+      <c r="U20">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="V20">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="W20">
+        <v>7.7439999999999995E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S25" t="s">
+        <v>10</v>
+      </c>
+      <c r="T25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>10</v>
+      </c>
+      <c r="S26">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="T26">
+        <v>0.371</v>
+      </c>
+    </row>
+    <row r="27" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>50</v>
+      </c>
+      <c r="S27">
+        <v>1.23E-2</v>
+      </c>
+      <c r="T27">
+        <v>0.23949999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>100</v>
+      </c>
+      <c r="S28">
+        <v>1.15E-2</v>
+      </c>
+      <c r="T28">
+        <v>0.18229999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>150</v>
+      </c>
+      <c r="S29">
+        <v>1.1599999999999999E-2</v>
+      </c>
+      <c r="T29">
+        <v>0.12239999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>200</v>
+      </c>
+      <c r="S30">
+        <v>1.06E-2</v>
+      </c>
+      <c r="T30">
+        <v>0.1303</v>
+      </c>
+    </row>
+    <row r="31" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>250</v>
+      </c>
+      <c r="S31">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="T31">
+        <v>8.8999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="18:23" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>300</v>
+      </c>
+      <c r="S32">
+        <v>0.01</v>
+      </c>
+      <c r="T32">
+        <v>8.2900000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>350</v>
+      </c>
+      <c r="S33">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="T33">
+        <v>7.2499999999999995E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R41" t="s">
+        <v>1</v>
+      </c>
+      <c r="S41" t="s">
+        <v>12</v>
+      </c>
+      <c r="T41" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>10</v>
+      </c>
+      <c r="S42">
+        <v>0.371</v>
+      </c>
+      <c r="T42">
+        <v>0.56499999999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>50</v>
+      </c>
+      <c r="S43">
+        <v>0.23949999999999999</v>
+      </c>
+      <c r="T43">
+        <v>0.51800000000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>100</v>
+      </c>
+      <c r="S44">
+        <v>0.18229999999999999</v>
+      </c>
+      <c r="T44">
+        <v>0.52500000000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>150</v>
+      </c>
+      <c r="S45">
+        <v>0.12239999999999999</v>
+      </c>
+      <c r="T45">
+        <v>0.49299999999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>200</v>
+      </c>
+      <c r="S46">
+        <v>0.1303</v>
+      </c>
+      <c r="T46">
+        <v>0.503</v>
+      </c>
+    </row>
+    <row r="47" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>250</v>
+      </c>
+      <c r="S47">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="T47">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="48" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>300</v>
+      </c>
+      <c r="S48">
+        <v>8.2900000000000001E-2</v>
+      </c>
+      <c r="T48">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="49" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>350</v>
+      </c>
+      <c r="S49">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="T49">
+        <v>0.497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 3000F, 3T result
</commit_message>
<xml_diff>
--- a/Paper/Experiments.xlsx
+++ b/Paper/Experiments.xlsx
@@ -408,11 +408,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96103424"/>
-        <c:axId val="96105600"/>
+        <c:axId val="111005056"/>
+        <c:axId val="111007232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96103424"/>
+        <c:axId val="111005056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,7 +441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96105600"/>
+        <c:crossAx val="111007232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -449,7 +449,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96105600"/>
+        <c:axId val="111007232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -481,7 +481,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96103424"/>
+        <c:crossAx val="111005056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -687,7 +687,7 @@
                   <c:v>0.12690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>9.4E-2</c:v>
@@ -713,11 +713,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100546816"/>
-        <c:axId val="100548992"/>
+        <c:axId val="116075520"/>
+        <c:axId val="116077696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100546816"/>
+        <c:axId val="116075520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -746,7 +746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100548992"/>
+        <c:crossAx val="116077696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -754,7 +754,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100548992"/>
+        <c:axId val="116077696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.4"/>
@@ -786,7 +786,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100546816"/>
+        <c:crossAx val="116075520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -926,11 +926,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="100565376"/>
-        <c:axId val="100567296"/>
+        <c:axId val="116110464"/>
+        <c:axId val="116112384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="100565376"/>
+        <c:axId val="116110464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -959,7 +959,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100567296"/>
+        <c:crossAx val="116112384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -967,7 +967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100567296"/>
+        <c:axId val="116112384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -999,7 +999,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="100565376"/>
+        <c:crossAx val="116110464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1702,11 +1702,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="105213312"/>
-        <c:axId val="105219584"/>
+        <c:axId val="116232576"/>
+        <c:axId val="116234496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="105213312"/>
+        <c:axId val="116232576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,7 +1735,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105219584"/>
+        <c:crossAx val="116234496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1743,7 +1743,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="105219584"/>
+        <c:axId val="116234496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -1775,7 +1775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105213312"/>
+        <c:crossAx val="116232576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1925,11 +1925,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="116587136"/>
-        <c:axId val="116622080"/>
+        <c:axId val="116251648"/>
+        <c:axId val="116262016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="116587136"/>
+        <c:axId val="116251648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1958,7 +1958,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116622080"/>
+        <c:crossAx val="116262016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1966,7 +1966,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116622080"/>
+        <c:axId val="116262016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -1998,7 +1998,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116587136"/>
+        <c:crossAx val="116251648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2148,11 +2148,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="113098112"/>
-        <c:axId val="113763840"/>
+        <c:axId val="116281344"/>
+        <c:axId val="116283264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="113098112"/>
+        <c:axId val="116281344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2181,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113763840"/>
+        <c:crossAx val="116283264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2189,7 +2189,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="113763840"/>
+        <c:axId val="116283264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.70000000000000007"/>
@@ -2221,7 +2221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="113098112"/>
+        <c:crossAx val="116281344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2310,15 +2310,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2728,7 +2728,7 @@
   <dimension ref="D1:W49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="O30" sqref="O30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,7 +2991,7 @@
         <v>0.1303</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="I6">
         <v>200</v>

</xml_diff>